<commit_message>
#44 fix text in config
</commit_message>
<xml_diff>
--- a/doc/Mapping.xlsx
+++ b/doc/Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\trest\Documents\solax\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trest\Source\Repos\HomeAssistant\homeassistant-solax-http\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E6DF37-CFA1-447F-8611-62151138B96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AA8D7D-5A40-438C-BB77-D9CE5524AAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E30620CE-52E2-4698-983C-BDD3AD23A8BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E30620CE-52E2-4698-983C-BDD3AD23A8BB}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>[</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Timezone</t>
   </si>
   <si>
-    <t>Firmware</t>
-  </si>
-  <si>
     <t>Main breaker limit</t>
   </si>
   <si>
@@ -211,6 +208,24 @@
   </si>
   <si>
     <t>!22 - reset charger</t>
+  </si>
+  <si>
+    <t>Slave baud rate</t>
+  </si>
+  <si>
+    <t>LCD language</t>
+  </si>
+  <si>
+    <t>Firmware/ Factory reset</t>
+  </si>
+  <si>
+    <t>/Reset</t>
+  </si>
+  <si>
+    <t>Current limit</t>
+  </si>
+  <si>
+    <t>Scene ??</t>
   </si>
 </sst>
 </file>
@@ -274,9 +289,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 –⁠ 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -314,7 +329,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 –⁠ 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -420,7 +435,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 –⁠ 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -562,7 +577,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -570,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E382A0D-967B-40F4-B1C8-B14BB77D210D}">
-  <dimension ref="A1:K71"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="L78" sqref="L78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,7 +598,7 @@
     <col min="5" max="5" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -597,7 +612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -628,8 +643,11 @@
       <c r="K2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -660,8 +678,11 @@
       <c r="K3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -692,8 +713,11 @@
       <c r="K4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -724,8 +748,11 @@
       <c r="K5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -756,8 +783,11 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -788,8 +818,11 @@
       <c r="K7">
         <v>265</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -820,8 +853,11 @@
       <c r="K8">
         <v>160</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -846,8 +882,11 @@
       <c r="K9">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -872,8 +911,11 @@
       <c r="K10">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -898,8 +940,11 @@
       <c r="K11">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -927,8 +972,11 @@
       <c r="K12">
         <v>12000</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -959,8 +1007,11 @@
       <c r="K13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -991,8 +1042,11 @@
       <c r="K14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1023,8 +1077,11 @@
       <c r="K15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1055,8 +1112,11 @@
       <c r="K16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1087,8 +1147,11 @@
       <c r="K17">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1113,8 +1176,11 @@
       <c r="K18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1145,16 +1211,19 @@
       <c r="K19">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
         <v>18</v>
       </c>
-      <c r="C20" t="s">
-        <v>46</v>
+      <c r="C20" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="D20">
         <v>70</v>
@@ -1177,16 +1246,19 @@
       <c r="K20">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D21">
         <v>108</v>
@@ -1209,8 +1281,11 @@
       <c r="K21">
         <v>108</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1235,11 +1310,17 @@
       <c r="K22">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
       <c r="D23">
         <v>0</v>
       </c>
@@ -1261,13 +1342,19 @@
       <c r="K23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1290,8 +1377,11 @@
       <c r="K24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1316,8 +1406,11 @@
       <c r="K25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1345,8 +1438,11 @@
       <c r="K26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1371,8 +1467,11 @@
       <c r="K27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1397,8 +1496,11 @@
       <c r="K28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1423,11 +1525,20 @@
       <c r="K29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
+      <c r="B30">
+        <v>28</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="D30">
         <v>0</v>
       </c>
@@ -1449,8 +1560,11 @@
       <c r="K30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1458,7 +1572,7 @@
         <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1481,8 +1595,11 @@
       <c r="K31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1490,7 +1607,7 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1513,8 +1630,11 @@
       <c r="K32">
         <v>12593</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1522,7 +1642,7 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1545,8 +1665,11 @@
       <c r="K33">
         <v>12593</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1554,7 +1677,7 @@
         <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -1577,8 +1700,11 @@
       <c r="K34">
         <v>12593</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1603,8 +1729,11 @@
       <c r="K35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1629,8 +1758,11 @@
       <c r="K36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1655,8 +1787,11 @@
       <c r="K37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1681,8 +1816,11 @@
       <c r="K38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1707,8 +1845,11 @@
       <c r="K39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1733,8 +1874,11 @@
       <c r="K40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1759,8 +1903,11 @@
       <c r="K41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1785,8 +1932,11 @@
       <c r="K42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1811,8 +1961,11 @@
       <c r="K43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1837,8 +1990,11 @@
       <c r="K44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1863,8 +2019,11 @@
       <c r="K45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1889,8 +2048,11 @@
       <c r="K46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1915,8 +2077,11 @@
       <c r="K47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1941,8 +2106,11 @@
       <c r="K48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1967,8 +2135,11 @@
       <c r="K49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1993,8 +2164,11 @@
       <c r="K50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2019,8 +2193,11 @@
       <c r="K51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2045,8 +2222,11 @@
       <c r="K52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2071,8 +2251,11 @@
       <c r="K53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2097,8 +2280,11 @@
       <c r="K54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2123,8 +2309,11 @@
       <c r="K55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2149,8 +2338,11 @@
       <c r="K56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2175,8 +2367,11 @@
       <c r="K57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2201,8 +2396,11 @@
       <c r="K58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -2227,8 +2425,11 @@
       <c r="K59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -2253,8 +2454,11 @@
       <c r="K60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -2279,8 +2483,11 @@
       <c r="K61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -2305,8 +2512,11 @@
       <c r="K62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -2331,8 +2541,11 @@
       <c r="K63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -2357,8 +2570,11 @@
       <c r="K64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -2383,8 +2599,11 @@
       <c r="K65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -2409,8 +2628,11 @@
       <c r="K66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -2418,7 +2640,7 @@
         <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -2441,8 +2663,11 @@
       <c r="K67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -2450,7 +2675,7 @@
         <v>71</v>
       </c>
       <c r="C68" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D68">
         <v>4600</v>
@@ -2473,8 +2698,11 @@
       <c r="K68">
         <v>4600</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L68">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -2482,7 +2710,7 @@
         <v>72</v>
       </c>
       <c r="C69" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -2505,8 +2733,11 @@
       <c r="K69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -2514,7 +2745,7 @@
         <v>73</v>
       </c>
       <c r="C70" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D70">
         <v>70</v>
@@ -2537,15 +2768,88 @@
       <c r="K70">
         <v>70</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B71" t="s">
-        <v>1</v>
-      </c>
-      <c r="E71" t="s">
-        <v>1</v>
-      </c>
-      <c r="G71" t="s">
+      <c r="L70">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="C76" t="s">
+        <v>57</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>75</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="L78">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="L79">
         <v>1</v>
       </c>
     </row>
@@ -2556,10 +2860,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8C0C25-584C-4DB3-91C9-D576A78C1B11}">
-  <dimension ref="A1:O98"/>
+  <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2567,12 +2871,12 @@
     <col min="2" max="2" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2618,8 +2922,11 @@
       <c r="O2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2665,8 +2972,11 @@
       <c r="O3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2712,8 +3022,11 @@
       <c r="O4">
         <v>23459</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4">
+        <v>23779</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2759,8 +3072,11 @@
       <c r="O5">
         <v>23518</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5">
+        <v>23734</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2806,8 +3122,11 @@
       <c r="O6">
         <v>23569</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6">
+        <v>23716</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2853,8 +3172,11 @@
       <c r="O7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2900,8 +3222,11 @@
       <c r="O8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2947,8 +3272,11 @@
       <c r="O9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2994,8 +3322,11 @@
       <c r="O10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3041,8 +3372,11 @@
       <c r="O11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3088,8 +3422,11 @@
       <c r="O12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3135,8 +3472,11 @@
       <c r="O13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3182,8 +3522,11 @@
       <c r="O14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3226,8 +3569,11 @@
       <c r="O15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3273,8 +3619,11 @@
       <c r="O16">
         <v>196</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16">
+        <v>12703</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3320,8 +3669,11 @@
       <c r="O17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3367,8 +3719,11 @@
       <c r="O18">
         <v>65457</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3414,8 +3769,11 @@
       <c r="O19">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P19">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3461,8 +3819,11 @@
       <c r="O20">
         <v>65468</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P20">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3508,8 +3869,11 @@
       <c r="O21">
         <v>65411</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P21">
+        <v>2245</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3555,8 +3919,11 @@
       <c r="O22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P22">
+        <v>2278</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3602,8 +3969,11 @@
       <c r="O23">
         <v>65531</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P23">
+        <v>2249</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3649,8 +4019,11 @@
       <c r="O24">
         <v>65409</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P24">
+        <v>6772</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3696,8 +4069,11 @@
       <c r="O25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3743,8 +4119,11 @@
       <c r="O26">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P26">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3787,8 +4166,11 @@
       <c r="O27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3834,8 +4216,11 @@
       <c r="O28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3878,8 +4263,11 @@
       <c r="O29">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3922,8 +4310,11 @@
       <c r="O30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3966,8 +4357,11 @@
       <c r="O31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -4010,8 +4404,11 @@
       <c r="O32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -4054,8 +4451,11 @@
       <c r="O33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -4098,8 +4498,11 @@
       <c r="O34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -4142,8 +4545,11 @@
       <c r="O35">
         <v>4994</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P35">
+        <v>4994</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -4186,8 +4592,11 @@
       <c r="O36">
         <v>4986</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P36">
+        <v>4990</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -4230,13 +4639,16 @@
       <c r="O37">
         <v>4998</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P37">
+        <v>4998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38">
         <v>10793</v>
@@ -4277,13 +4689,16 @@
       <c r="O38">
         <v>5153</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P38">
+        <v>6422</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39">
         <v>5141</v>
@@ -4324,13 +4739,16 @@
       <c r="O39">
         <v>5643</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P39">
+        <v>6924</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40">
         <v>5899</v>
@@ -4371,8 +4789,11 @@
       <c r="O40">
         <v>5899</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P40">
+        <v>6150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -4415,8 +4836,11 @@
       <c r="O41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -4459,8 +4883,11 @@
       <c r="O42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -4503,8 +4930,11 @@
       <c r="O43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -4547,8 +4977,11 @@
       <c r="O44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -4591,8 +5024,11 @@
       <c r="O45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -4635,8 +5071,11 @@
       <c r="O46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -4679,8 +5118,11 @@
       <c r="O47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -4723,8 +5165,11 @@
       <c r="O48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -4767,8 +5212,11 @@
       <c r="O49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -4811,8 +5259,11 @@
       <c r="O50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -4855,8 +5306,11 @@
       <c r="O51">
         <v>100</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P51">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -4899,8 +5353,11 @@
       <c r="O52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -4943,8 +5400,11 @@
       <c r="O53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -4987,8 +5447,11 @@
       <c r="O54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -5031,8 +5494,11 @@
       <c r="O55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -5075,8 +5541,11 @@
       <c r="O56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -5119,8 +5588,11 @@
       <c r="O57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -5163,8 +5635,11 @@
       <c r="O58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -5207,8 +5682,11 @@
       <c r="O59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -5251,8 +5729,11 @@
       <c r="O60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -5295,8 +5776,11 @@
       <c r="O61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -5339,8 +5823,11 @@
       <c r="O62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -5383,8 +5870,11 @@
       <c r="O63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -5427,8 +5917,11 @@
       <c r="O64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -5471,8 +5964,11 @@
       <c r="O65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -5515,8 +6011,11 @@
       <c r="O66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -5559,8 +6058,11 @@
       <c r="O67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -5603,8 +6105,11 @@
       <c r="O68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -5647,8 +6152,11 @@
       <c r="O69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -5691,8 +6199,11 @@
       <c r="O70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -5735,8 +6246,11 @@
       <c r="O71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -5779,8 +6293,11 @@
       <c r="O72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -5823,8 +6340,11 @@
       <c r="O73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
@@ -5867,8 +6387,11 @@
       <c r="O74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -5911,8 +6434,11 @@
       <c r="O75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -5955,8 +6481,11 @@
       <c r="O76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -5999,8 +6528,11 @@
       <c r="O77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -6043,8 +6575,11 @@
       <c r="O78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -6087,8 +6622,11 @@
       <c r="O79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
@@ -6131,8 +6669,11 @@
       <c r="O80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
@@ -6175,8 +6716,11 @@
       <c r="O81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
@@ -6222,8 +6766,11 @@
       <c r="O82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
@@ -6269,8 +6816,11 @@
       <c r="O83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
@@ -6313,8 +6863,11 @@
       <c r="O84">
         <v>12318</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P84">
+        <v>13317</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -6357,8 +6910,11 @@
       <c r="O85">
         <v>5141</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P85">
+        <v>6667</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
@@ -6401,8 +6957,11 @@
       <c r="O86">
         <v>5899</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P86">
+        <v>6150</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
@@ -6448,8 +7007,11 @@
       <c r="O87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
@@ -6492,8 +7054,11 @@
       <c r="O88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
@@ -6539,8 +7104,11 @@
       <c r="O89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
@@ -6586,8 +7154,11 @@
       <c r="O90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
@@ -6633,8 +7204,11 @@
       <c r="O91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
@@ -6677,8 +7251,11 @@
       <c r="O92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
@@ -6721,8 +7298,11 @@
       <c r="O93">
         <v>120</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P93">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
@@ -6765,8 +7345,11 @@
       <c r="O94">
         <v>1195</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P94">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
@@ -6809,8 +7392,11 @@
       <c r="O95">
         <v>1000</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P95">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
@@ -6853,8 +7439,11 @@
       <c r="O96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
@@ -6897,8 +7486,11 @@
       <c r="O97">
         <v>44</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P97">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Mapping first Options for G2 (read only)
</commit_message>
<xml_diff>
--- a/doc/Mapping.xlsx
+++ b/doc/Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trest\Source\Repos\HomeAssistant\homeassistant-solax-http\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2838EAF1-CCBD-4308-ABA1-3C624A5C1895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A71BBE2-99C7-4A16-A8D7-ADF728575030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E30620CE-52E2-4698-983C-BDD3AD23A8BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E30620CE-52E2-4698-983C-BDD3AD23A8BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="71">
   <si>
     <t>[</t>
   </si>
@@ -183,9 +183,6 @@
     <t>/Reset</t>
   </si>
   <si>
-    <t>Current limit</t>
-  </si>
-  <si>
     <t>Scene ??</t>
   </si>
   <si>
@@ -250,6 +247,9 @@
   </si>
   <si>
     <t>Something with PV??</t>
+  </si>
+  <si>
+    <t>Max Charge Current</t>
   </si>
 </sst>
 </file>
@@ -612,34 +612,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E382A0D-967B-40F4-B1C8-B14BB77D210D}">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:N87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.21875" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -652,6 +649,9 @@
       <c r="D2">
         <v>2</v>
       </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
       <c r="F2">
         <v>2</v>
       </c>
@@ -670,11 +670,11 @@
       <c r="K2">
         <v>2</v>
       </c>
-      <c r="L2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -687,17 +687,20 @@
       <c r="D3">
         <v>1</v>
       </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
       <c r="F3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -705,11 +708,11 @@
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -722,6 +725,9 @@
       <c r="D4">
         <v>6</v>
       </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
       <c r="F4">
         <v>6</v>
       </c>
@@ -740,11 +746,14 @@
       <c r="K4">
         <v>6</v>
       </c>
-      <c r="L4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4">
+        <v>70</v>
+      </c>
+      <c r="N4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -757,6 +766,9 @@
       <c r="D5">
         <v>6</v>
       </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
       <c r="F5">
         <v>6</v>
       </c>
@@ -773,13 +785,16 @@
         <v>6</v>
       </c>
       <c r="K5">
-        <v>6</v>
-      </c>
-      <c r="L5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>16</v>
+      </c>
+      <c r="N5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -792,11 +807,14 @@
       <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -810,11 +828,11 @@
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -827,6 +845,9 @@
       <c r="D7">
         <v>265</v>
       </c>
+      <c r="E7">
+        <v>265</v>
+      </c>
       <c r="F7">
         <v>265</v>
       </c>
@@ -845,11 +866,11 @@
       <c r="K7">
         <v>265</v>
       </c>
-      <c r="L7">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -862,6 +883,9 @@
       <c r="D8">
         <v>160</v>
       </c>
+      <c r="E8">
+        <v>160</v>
+      </c>
       <c r="F8">
         <v>160</v>
       </c>
@@ -880,17 +904,20 @@
       <c r="K8">
         <v>160</v>
       </c>
-      <c r="L8">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="D9">
         <v>18</v>
       </c>
+      <c r="E9">
+        <v>18</v>
+      </c>
       <c r="F9">
         <v>18</v>
       </c>
@@ -909,17 +936,20 @@
       <c r="K9">
         <v>18</v>
       </c>
-      <c r="L9">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="D10">
         <v>80</v>
       </c>
+      <c r="E10">
+        <v>80</v>
+      </c>
       <c r="F10">
         <v>80</v>
       </c>
@@ -938,17 +968,20 @@
       <c r="K10">
         <v>80</v>
       </c>
-      <c r="L10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="D11">
         <v>30</v>
       </c>
+      <c r="E11">
+        <v>30</v>
+      </c>
       <c r="F11">
         <v>30</v>
       </c>
@@ -967,11 +1000,11 @@
       <c r="K11">
         <v>30</v>
       </c>
-      <c r="L11">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -980,18 +1013,20 @@
       <c r="D12" s="1">
         <v>8000</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>8000</v>
+      </c>
       <c r="F12" s="1">
+        <v>12000</v>
+      </c>
+      <c r="G12">
         <v>8000</v>
-      </c>
-      <c r="G12" s="1">
-        <v>12000</v>
       </c>
       <c r="H12">
         <v>8000</v>
       </c>
       <c r="I12">
-        <v>8000</v>
+        <v>12000</v>
       </c>
       <c r="J12">
         <v>12000</v>
@@ -999,11 +1034,11 @@
       <c r="K12">
         <v>12000</v>
       </c>
-      <c r="L12">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1016,6 +1051,9 @@
       <c r="D13">
         <v>0</v>
       </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
       <c r="F13">
         <v>0</v>
       </c>
@@ -1034,11 +1072,11 @@
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1051,6 +1089,9 @@
       <c r="D14">
         <v>0</v>
       </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
       <c r="F14">
         <v>0</v>
       </c>
@@ -1069,11 +1110,11 @@
       <c r="K14">
         <v>0</v>
       </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1086,6 +1127,9 @@
       <c r="D15">
         <v>0</v>
       </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
       <c r="F15">
         <v>0</v>
       </c>
@@ -1104,11 +1148,14 @@
       <c r="K15">
         <v>0</v>
       </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15">
+        <v>265</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1121,6 +1168,9 @@
       <c r="D16">
         <v>0</v>
       </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
       <c r="F16">
         <v>0</v>
       </c>
@@ -1139,11 +1189,14 @@
       <c r="K16">
         <v>0</v>
       </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16">
+        <v>160</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1156,11 +1209,14 @@
       <c r="D17">
         <v>0</v>
       </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H17">
         <v>50</v>
@@ -1172,19 +1228,22 @@
         <v>50</v>
       </c>
       <c r="K17">
-        <v>50</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
       <c r="F18">
         <v>0</v>
       </c>
@@ -1203,11 +1262,11 @@
       <c r="K18">
         <v>0</v>
       </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1220,6 +1279,9 @@
       <c r="D19">
         <v>44</v>
       </c>
+      <c r="E19">
+        <v>44</v>
+      </c>
       <c r="F19">
         <v>44</v>
       </c>
@@ -1238,28 +1300,31 @@
       <c r="K19">
         <v>44</v>
       </c>
-      <c r="L19">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
         <v>18</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>48</v>
+      <c r="C20" t="s">
+        <v>32</v>
       </c>
       <c r="D20">
         <v>70</v>
       </c>
+      <c r="E20">
+        <v>70</v>
+      </c>
       <c r="F20">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G20">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="H20">
         <v>50</v>
@@ -1271,13 +1336,13 @@
         <v>50</v>
       </c>
       <c r="K20">
-        <v>50</v>
-      </c>
-      <c r="L20">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1290,6 +1355,9 @@
       <c r="D21">
         <v>108</v>
       </c>
+      <c r="E21">
+        <v>108</v>
+      </c>
       <c r="F21">
         <v>108</v>
       </c>
@@ -1306,19 +1374,22 @@
         <v>108</v>
       </c>
       <c r="K21">
-        <v>108</v>
-      </c>
-      <c r="L21">
         <v>112</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="D22">
         <v>101</v>
       </c>
+      <c r="E22">
+        <v>101</v>
+      </c>
       <c r="F22">
         <v>101</v>
       </c>
@@ -1337,11 +1408,11 @@
       <c r="K22">
         <v>101</v>
       </c>
-      <c r="L22">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1351,6 +1422,9 @@
       <c r="D23">
         <v>0</v>
       </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
       <c r="F23">
         <v>0</v>
       </c>
@@ -1369,11 +1443,14 @@
       <c r="K23">
         <v>0</v>
       </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M23">
+        <v>44</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1386,6 +1463,9 @@
       <c r="D24">
         <v>0</v>
       </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
       <c r="F24">
         <v>0</v>
       </c>
@@ -1404,17 +1484,20 @@
       <c r="K24">
         <v>0</v>
       </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M24">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
       <c r="F25">
         <v>0</v>
       </c>
@@ -1433,11 +1516,11 @@
       <c r="K25">
         <v>0</v>
       </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1447,6 +1530,9 @@
       <c r="D26">
         <v>0</v>
       </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
       <c r="F26">
         <v>0</v>
       </c>
@@ -1460,22 +1546,25 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26">
-        <v>1</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
       <c r="F27">
         <v>0</v>
       </c>
@@ -1494,17 +1583,23 @@
       <c r="K27">
         <v>0</v>
       </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M27">
+        <v>12593</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
       <c r="F28">
         <v>0</v>
       </c>
@@ -1523,17 +1618,23 @@
       <c r="K28">
         <v>0</v>
       </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M28">
+        <v>12593</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
       <c r="F29">
         <v>0</v>
       </c>
@@ -1552,11 +1653,14 @@
       <c r="K29">
         <v>0</v>
       </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M29">
+        <v>12593</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1564,11 +1668,14 @@
         <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
       <c r="F30">
         <v>0</v>
       </c>
@@ -1587,11 +1694,11 @@
       <c r="K30">
         <v>0</v>
       </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1604,11 +1711,14 @@
       <c r="D31">
         <v>0</v>
       </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
       <c r="F31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -1622,11 +1732,11 @@
       <c r="K31">
         <v>0</v>
       </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1639,8 +1749,11 @@
       <c r="D32">
         <v>0</v>
       </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
       <c r="F32">
-        <v>0</v>
+        <v>12593</v>
       </c>
       <c r="G32">
         <v>12593</v>
@@ -1655,13 +1768,13 @@
         <v>12593</v>
       </c>
       <c r="K32">
-        <v>12593</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1674,8 +1787,11 @@
       <c r="D33">
         <v>0</v>
       </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
       <c r="F33">
-        <v>0</v>
+        <v>12593</v>
       </c>
       <c r="G33">
         <v>12593</v>
@@ -1690,13 +1806,13 @@
         <v>12593</v>
       </c>
       <c r="K33">
-        <v>12593</v>
-      </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1709,8 +1825,11 @@
       <c r="D34">
         <v>0</v>
       </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
       <c r="F34">
-        <v>0</v>
+        <v>12593</v>
       </c>
       <c r="G34">
         <v>12593</v>
@@ -1725,19 +1844,22 @@
         <v>12593</v>
       </c>
       <c r="K34">
-        <v>12593</v>
-      </c>
-      <c r="L34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
       <c r="F35">
         <v>0</v>
       </c>
@@ -1756,17 +1878,20 @@
       <c r="K35">
         <v>0</v>
       </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
       <c r="F36">
         <v>0</v>
       </c>
@@ -1785,17 +1910,20 @@
       <c r="K36">
         <v>0</v>
       </c>
-      <c r="L36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
       <c r="F37">
         <v>0</v>
       </c>
@@ -1814,17 +1942,20 @@
       <c r="K37">
         <v>0</v>
       </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
       <c r="F38">
         <v>0</v>
       </c>
@@ -1843,17 +1974,20 @@
       <c r="K38">
         <v>0</v>
       </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
       <c r="F39">
         <v>0</v>
       </c>
@@ -1872,17 +2006,20 @@
       <c r="K39">
         <v>0</v>
       </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
       <c r="F40">
         <v>0</v>
       </c>
@@ -1901,17 +2038,20 @@
       <c r="K40">
         <v>0</v>
       </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
       <c r="F41">
         <v>0</v>
       </c>
@@ -1930,17 +2070,20 @@
       <c r="K41">
         <v>0</v>
       </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
       <c r="F42">
         <v>0</v>
       </c>
@@ -1959,17 +2102,20 @@
       <c r="K42">
         <v>0</v>
       </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
       <c r="F43">
         <v>0</v>
       </c>
@@ -1988,17 +2134,20 @@
       <c r="K43">
         <v>0</v>
       </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
       <c r="F44">
         <v>0</v>
       </c>
@@ -2017,17 +2166,20 @@
       <c r="K44">
         <v>0</v>
       </c>
-      <c r="L44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
       <c r="F45">
         <v>0</v>
       </c>
@@ -2046,17 +2198,20 @@
       <c r="K45">
         <v>0</v>
       </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
       <c r="F46">
         <v>0</v>
       </c>
@@ -2075,17 +2230,20 @@
       <c r="K46">
         <v>0</v>
       </c>
-      <c r="L46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
       <c r="F47">
         <v>0</v>
       </c>
@@ -2104,17 +2262,20 @@
       <c r="K47">
         <v>0</v>
       </c>
-      <c r="L47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M47">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
       <c r="F48">
         <v>0</v>
       </c>
@@ -2133,17 +2294,20 @@
       <c r="K48">
         <v>0</v>
       </c>
-      <c r="L48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
       <c r="F49">
         <v>0</v>
       </c>
@@ -2162,17 +2326,20 @@
       <c r="K49">
         <v>0</v>
       </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
       <c r="F50">
         <v>0</v>
       </c>
@@ -2191,17 +2358,20 @@
       <c r="K50">
         <v>0</v>
       </c>
-      <c r="L50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
       <c r="F51">
         <v>0</v>
       </c>
@@ -2220,17 +2390,20 @@
       <c r="K51">
         <v>0</v>
       </c>
-      <c r="L51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
       <c r="F52">
         <v>0</v>
       </c>
@@ -2249,17 +2422,20 @@
       <c r="K52">
         <v>0</v>
       </c>
-      <c r="L52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
       <c r="F53">
         <v>0</v>
       </c>
@@ -2278,17 +2454,20 @@
       <c r="K53">
         <v>0</v>
       </c>
-      <c r="L53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
       <c r="F54">
         <v>0</v>
       </c>
@@ -2307,17 +2486,20 @@
       <c r="K54">
         <v>0</v>
       </c>
-      <c r="L54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
       <c r="F55">
         <v>0</v>
       </c>
@@ -2336,17 +2518,20 @@
       <c r="K55">
         <v>0</v>
       </c>
-      <c r="L55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="D56">
         <v>0</v>
       </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
       <c r="F56">
         <v>0</v>
       </c>
@@ -2365,17 +2550,20 @@
       <c r="K56">
         <v>0</v>
       </c>
-      <c r="L56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="D57">
         <v>0</v>
       </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
       <c r="F57">
         <v>0</v>
       </c>
@@ -2394,17 +2582,20 @@
       <c r="K57">
         <v>0</v>
       </c>
-      <c r="L57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="D58">
         <v>0</v>
       </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
       <c r="F58">
         <v>0</v>
       </c>
@@ -2423,17 +2614,20 @@
       <c r="K58">
         <v>0</v>
       </c>
-      <c r="L58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="D59">
         <v>0</v>
       </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
       <c r="F59">
         <v>0</v>
       </c>
@@ -2452,17 +2646,20 @@
       <c r="K59">
         <v>0</v>
       </c>
-      <c r="L59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="D60">
         <v>0</v>
       </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
       <c r="F60">
         <v>0</v>
       </c>
@@ -2481,17 +2678,20 @@
       <c r="K60">
         <v>0</v>
       </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="D61">
         <v>0</v>
       </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
       <c r="F61">
         <v>0</v>
       </c>
@@ -2510,17 +2710,20 @@
       <c r="K61">
         <v>0</v>
       </c>
-      <c r="L61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
       <c r="F62">
         <v>0</v>
       </c>
@@ -2539,17 +2742,20 @@
       <c r="K62">
         <v>0</v>
       </c>
-      <c r="L62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
       <c r="F63">
         <v>0</v>
       </c>
@@ -2568,17 +2774,20 @@
       <c r="K63">
         <v>0</v>
       </c>
-      <c r="L63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
       <c r="D64">
         <v>0</v>
       </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
       <c r="F64">
         <v>0</v>
       </c>
@@ -2597,17 +2806,20 @@
       <c r="K64">
         <v>0</v>
       </c>
-      <c r="L64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="D65">
         <v>0</v>
       </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
       <c r="F65">
         <v>0</v>
       </c>
@@ -2626,17 +2838,20 @@
       <c r="K65">
         <v>0</v>
       </c>
-      <c r="L65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="D66">
         <v>0</v>
       </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
       <c r="F66">
         <v>0</v>
       </c>
@@ -2655,11 +2870,11 @@
       <c r="K66">
         <v>0</v>
       </c>
-      <c r="L66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -2672,6 +2887,9 @@
       <c r="D67">
         <v>0</v>
       </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
       <c r="F67">
         <v>0</v>
       </c>
@@ -2690,11 +2908,11 @@
       <c r="K67">
         <v>0</v>
       </c>
-      <c r="L67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -2707,6 +2925,9 @@
       <c r="D68">
         <v>4600</v>
       </c>
+      <c r="E68">
+        <v>4600</v>
+      </c>
       <c r="F68">
         <v>4600</v>
       </c>
@@ -2725,11 +2946,11 @@
       <c r="K68">
         <v>4600</v>
       </c>
-      <c r="L68">
-        <v>4600</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -2742,6 +2963,9 @@
       <c r="D69">
         <v>0</v>
       </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
       <c r="F69">
         <v>0</v>
       </c>
@@ -2760,11 +2984,11 @@
       <c r="K69">
         <v>0</v>
       </c>
-      <c r="L69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -2777,6 +3001,9 @@
       <c r="D70">
         <v>70</v>
       </c>
+      <c r="E70">
+        <v>70</v>
+      </c>
       <c r="F70">
         <v>70</v>
       </c>
@@ -2795,62 +3022,83 @@
       <c r="K70">
         <v>70</v>
       </c>
-      <c r="L70">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
-      <c r="L71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
-      <c r="L72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
-      <c r="L73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>4600</v>
+      </c>
+      <c r="N73" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
-      <c r="L74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
-      <c r="L75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
       <c r="C76" t="s">
         <v>44</v>
       </c>
-      <c r="L76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K76">
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -2860,28 +3108,84 @@
       <c r="C77" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K77">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
-      <c r="L78">
+      <c r="B78">
+        <v>82</v>
+      </c>
+      <c r="C78" t="s">
+        <v>70</v>
+      </c>
+      <c r="K78">
         <v>16</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
-      <c r="L79">
+      <c r="K79">
         <v>1</v>
+      </c>
+      <c r="M79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M80">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="81" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M86">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="87" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M87">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2889,7 +3193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8C0C25-584C-4DB3-91C9-D576A78C1B11}">
   <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -2902,16 +3206,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -2968,7 +3272,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4">
         <v>23488</v>
@@ -2991,7 +3295,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5">
         <v>23535</v>
@@ -3009,7 +3313,7 @@
         <v>23382</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -3017,7 +3321,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6">
         <v>23606</v>
@@ -3035,7 +3339,7 @@
         <v>23225</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -3043,7 +3347,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -3061,7 +3365,7 @@
         <v>23300</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -3069,7 +3373,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -3087,7 +3391,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -3095,7 +3399,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -3113,7 +3417,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -3121,7 +3425,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -3139,7 +3443,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -3147,7 +3451,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -3165,7 +3469,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -3173,7 +3477,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -3191,7 +3495,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -3217,7 +3521,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -3225,7 +3529,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -3271,7 +3575,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16">
         <v>196</v>
@@ -3294,7 +3598,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -3312,7 +3616,7 @@
         <v>4</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -3338,7 +3642,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -3461,7 +3765,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24">
         <v>65395</v>
@@ -3699,7 +4003,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C35">
         <v>4992</v>
@@ -3717,7 +4021,7 @@
         <v>4984</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -3725,7 +4029,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C36">
         <v>4984</v>
@@ -3743,7 +4047,7 @@
         <v>4988</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -3751,7 +4055,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C37">
         <v>4996</v>
@@ -3769,7 +4073,7 @@
         <v>4984</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -4722,7 +5026,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C84">
         <v>12318</v>
@@ -4923,7 +5227,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C93">
         <v>120</v>
@@ -4946,7 +5250,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C94">
         <v>1195</v>
@@ -4969,7 +5273,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C95">
         <v>1000</v>

</xml_diff>

<commit_message>
#52 adding X1 7kW type
</commit_message>
<xml_diff>
--- a/doc/Mapping.xlsx
+++ b/doc/Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trest\Source\Repos\HomeAssistant\homeassistant-solax-http\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A71BBE2-99C7-4A16-A8D7-ADF728575030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA50947-1282-468F-A5F3-5DC08695C10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E30620CE-52E2-4698-983C-BDD3AD23A8BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E30620CE-52E2-4698-983C-BDD3AD23A8BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
   <si>
     <t>[</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Max Charge Current</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
@@ -266,7 +269,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,6 +279,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,12 +307,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -614,15 +632,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E382A0D-967B-40F4-B1C8-B14BB77D210D}">
   <dimension ref="A1:N87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="P73" sqref="P73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.21875" customWidth="1"/>
-    <col min="14" max="14" width="13.109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -711,6 +729,9 @@
       <c r="M3">
         <v>0</v>
       </c>
+      <c r="N3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -749,7 +770,7 @@
       <c r="M4">
         <v>70</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -790,7 +811,7 @@
       <c r="M5">
         <v>16</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1151,7 +1172,7 @@
       <c r="M15">
         <v>265</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="N15" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1192,7 +1213,7 @@
       <c r="M16">
         <v>160</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="N16" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1446,7 +1467,7 @@
       <c r="M23">
         <v>44</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="N23" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1586,7 +1607,7 @@
       <c r="M27">
         <v>12593</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="N27" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1621,7 +1642,7 @@
       <c r="M28">
         <v>12593</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="N28" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1656,7 +1677,7 @@
       <c r="M29">
         <v>12593</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="N29" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3058,7 +3079,7 @@
       <c r="M73">
         <v>4600</v>
       </c>
-      <c r="N73" s="1" t="s">
+      <c r="N73" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3193,15 +3214,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8C0C25-584C-4DB3-91C9-D576A78C1B11}">
   <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="8" max="8" width="10.77734375" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -3240,8 +3261,8 @@
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>1</v>
+      <c r="J2" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -3289,6 +3310,9 @@
       <c r="H4">
         <v>0</v>
       </c>
+      <c r="J4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -3312,7 +3336,7 @@
       <c r="H5">
         <v>23382</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="3" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3338,7 +3362,7 @@
       <c r="H6">
         <v>23225</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3364,7 +3388,7 @@
       <c r="H7">
         <v>23300</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3390,7 +3414,7 @@
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3416,7 +3440,7 @@
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="3" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3442,7 +3466,7 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="3" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3468,7 +3492,7 @@
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="3" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3494,7 +3518,7 @@
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3520,7 +3544,7 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="3" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3546,7 +3570,7 @@
       <c r="H14">
         <v>0</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3615,7 +3639,7 @@
       <c r="H17">
         <v>4</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="3" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3641,7 +3665,7 @@
       <c r="H18">
         <v>0</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="3" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3828,7 +3852,7 @@
       <c r="H26">
         <v>15</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="J26" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3851,7 +3875,7 @@
       <c r="H27">
         <v>21</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="J27" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -4020,7 +4044,7 @@
       <c r="H35">
         <v>4984</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="J35" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4046,7 +4070,7 @@
       <c r="H36">
         <v>4988</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="J36" s="3" t="s">
         <v>66</v>
       </c>
     </row>
@@ -4072,7 +4096,7 @@
       <c r="H37">
         <v>4984</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="J37" s="3" t="s">
         <v>67</v>
       </c>
     </row>
@@ -4098,7 +4122,7 @@
       <c r="H38">
         <v>13074</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="J38" s="3" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4124,7 +4148,7 @@
       <c r="H39">
         <v>1810</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="J39" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4150,7 +4174,7 @@
       <c r="H40">
         <v>6155</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="J40" s="3" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix Charger USe Mode reading #56
</commit_message>
<xml_diff>
--- a/doc/Mapping.xlsx
+++ b/doc/Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trest\Source\Repos\HomeAssistant\homeassistant-solax-http\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA50947-1282-468F-A5F3-5DC08695C10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60824D9-C86F-4332-AC91-FA0805E9BD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E30620CE-52E2-4698-983C-BDD3AD23A8BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E30620CE-52E2-4698-983C-BDD3AD23A8BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="140">
   <si>
     <t>[</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Charge time</t>
   </si>
   <si>
-    <t>OCPP offline</t>
-  </si>
-  <si>
     <t>Type power</t>
   </si>
   <si>
@@ -253,13 +250,220 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>unplugged</t>
+  </si>
+  <si>
+    <t>stopped</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Eco</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>SceneValue</t>
+  </si>
+  <si>
+    <t>chargingPhase</t>
+  </si>
+  <si>
+    <t>threePhaseInput</t>
+  </si>
+  <si>
+    <t>threePhaseSelect</t>
+  </si>
+  <si>
+    <t>ParallelSettingValue</t>
+  </si>
+  <si>
+    <t>SecondaryNumber</t>
+  </si>
+  <si>
+    <t>masterSlaveRatioValue</t>
+  </si>
+  <si>
+    <t>delayStartSwitch</t>
+  </si>
+  <si>
+    <t>delayDuration</t>
+  </si>
+  <si>
+    <t>GridType</t>
+  </si>
+  <si>
+    <t>OverVoltage</t>
+  </si>
+  <si>
+    <t>LowVoltage</t>
+  </si>
+  <si>
+    <t>Charging_pile_status</t>
+  </si>
+  <si>
+    <t>EVSE_Scene</t>
+  </si>
+  <si>
+    <t>Solar_Mode</t>
+  </si>
+  <si>
+    <t>Total_ChargePower</t>
+  </si>
+  <si>
+    <t>EQ_Single</t>
+  </si>
+  <si>
+    <t>MainBreakerLimitState</t>
+  </si>
+  <si>
+    <t>Extern_CurrentA</t>
+  </si>
+  <si>
+    <t>Extern_CurrentB</t>
+  </si>
+  <si>
+    <t>Extern_CurrentC</t>
+  </si>
+  <si>
+    <t>Extern_PowerA</t>
+  </si>
+  <si>
+    <t>Extern_PowerB</t>
+  </si>
+  <si>
+    <t>Extern_PowerC</t>
+  </si>
+  <si>
+    <t>Extern_TotalPower</t>
+  </si>
+  <si>
+    <t>CC_State</t>
+  </si>
+  <si>
+    <t>CP_State</t>
+  </si>
+  <si>
+    <t>Fault_Code</t>
+  </si>
+  <si>
+    <t>Q_Save_Single</t>
+  </si>
+  <si>
+    <t>EQ_Save_Total</t>
+  </si>
+  <si>
+    <t>RTC_WeekDay</t>
+  </si>
+  <si>
+    <t>Lock_Status</t>
+  </si>
+  <si>
+    <t>ChargingDuration</t>
+  </si>
+  <si>
+    <t>Start_Seconds/Min</t>
+  </si>
+  <si>
+    <t>Start_Hours/Days</t>
+  </si>
+  <si>
+    <t>Start_Months/Years</t>
+  </si>
+  <si>
+    <t>CC_value</t>
+  </si>
+  <si>
+    <t>CP_value</t>
+  </si>
+  <si>
+    <t>CP_PWM</t>
+  </si>
+  <si>
+    <t>TimeDifference</t>
+  </si>
+  <si>
+    <t>area_code</t>
+  </si>
+  <si>
+    <t>delay_state</t>
+  </si>
+  <si>
+    <t>schedule_state</t>
+  </si>
+  <si>
+    <t>Network_state</t>
+  </si>
+  <si>
+    <t>Authen_required</t>
+  </si>
+  <si>
+    <t>OCPP_Meter_Type</t>
+  </si>
+  <si>
+    <t>L1NRelay_Open_Time</t>
+  </si>
+  <si>
+    <t>L1NRelay_Close_Time</t>
+  </si>
+  <si>
+    <t>L1L2Relay_Open_Time</t>
+  </si>
+  <si>
+    <t>L1L2Relay_Close_Time</t>
+  </si>
+  <si>
+    <t>OCPP_Meter_Ua</t>
+  </si>
+  <si>
+    <t>OCPP_Meter_Ub</t>
+  </si>
+  <si>
+    <t>OCPP_Meter_Uc</t>
+  </si>
+  <si>
+    <t>Charger_scene</t>
+  </si>
+  <si>
+    <t>Type_screen</t>
+  </si>
+  <si>
+    <t>GreenGear</t>
+  </si>
+  <si>
+    <t>ECOGear</t>
+  </si>
+  <si>
+    <t>FASTGear</t>
+  </si>
+  <si>
+    <t>PrivateMode</t>
+  </si>
+  <si>
+    <t>StartTime</t>
+  </si>
+  <si>
+    <t>EndTime</t>
+  </si>
+  <si>
+    <t>Set_EQValue</t>
+  </si>
+  <si>
+    <t>Set_TimeValue</t>
+  </si>
+  <si>
+    <t>boostMode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,8 +472,15 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,6 +505,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -307,15 +524,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -630,31 +850,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E382A0D-967B-40F4-B1C8-B14BB77D210D}">
-  <dimension ref="A1:N87"/>
+  <dimension ref="A1:W87"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="P73" sqref="P73"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.21875" customWidth="1"/>
-    <col min="14" max="14" width="13.109375" style="5" customWidth="1"/>
+    <col min="14" max="18" width="13.109375" customWidth="1"/>
+    <col min="19" max="19" width="13.109375" style="3" customWidth="1"/>
+    <col min="22" max="22" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -662,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -691,8 +931,29 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -729,11 +990,33 @@
       <c r="M3">
         <v>0</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="R3">
+        <v>3</v>
+      </c>
+      <c r="S3"/>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3" t="s">
+        <v>2</v>
+      </c>
+      <c r="W3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -741,7 +1024,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -770,11 +1053,29 @@
       <c r="M4">
         <v>70</v>
       </c>
-      <c r="N4" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N4">
+        <v>70</v>
+      </c>
+      <c r="O4">
+        <v>70</v>
+      </c>
+      <c r="P4">
+        <v>70</v>
+      </c>
+      <c r="Q4">
+        <v>70</v>
+      </c>
+      <c r="R4">
+        <v>70</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="U4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -782,7 +1083,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -811,11 +1112,35 @@
       <c r="M5">
         <v>16</v>
       </c>
-      <c r="N5" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N5">
+        <v>16</v>
+      </c>
+      <c r="O5">
+        <v>16</v>
+      </c>
+      <c r="P5">
+        <v>16</v>
+      </c>
+      <c r="Q5">
+        <v>16</v>
+      </c>
+      <c r="R5">
+        <v>16</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="U5">
+        <v>3</v>
+      </c>
+      <c r="V5" t="s">
+        <v>133</v>
+      </c>
+      <c r="W5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -823,7 +1148,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -852,8 +1177,29 @@
       <c r="M6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>4</v>
+      </c>
+      <c r="V6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -861,7 +1207,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <v>265</v>
@@ -890,8 +1236,26 @@
       <c r="M7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -899,7 +1263,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>160</v>
@@ -928,8 +1292,26 @@
       <c r="M8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -960,8 +1342,26 @@
       <c r="M9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -992,8 +1392,26 @@
       <c r="M10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1024,8 +1442,26 @@
       <c r="M11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1058,8 +1494,26 @@
       <c r="M12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="U12" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1067,7 +1521,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1096,8 +1550,32 @@
       <c r="M13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N13">
+        <v>10</v>
+      </c>
+      <c r="O13">
+        <v>10</v>
+      </c>
+      <c r="P13">
+        <v>10</v>
+      </c>
+      <c r="Q13">
+        <v>10</v>
+      </c>
+      <c r="R13">
+        <v>10</v>
+      </c>
+      <c r="U13">
+        <v>11</v>
+      </c>
+      <c r="V13" t="s">
+        <v>132</v>
+      </c>
+      <c r="W13">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1105,7 +1583,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1134,8 +1612,32 @@
       <c r="M14">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N14">
+        <v>6</v>
+      </c>
+      <c r="O14">
+        <v>6</v>
+      </c>
+      <c r="P14">
+        <v>6</v>
+      </c>
+      <c r="Q14">
+        <v>6</v>
+      </c>
+      <c r="R14">
+        <v>6</v>
+      </c>
+      <c r="U14">
+        <v>12</v>
+      </c>
+      <c r="V14" t="s">
+        <v>131</v>
+      </c>
+      <c r="W14">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1143,7 +1645,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1172,11 +1674,35 @@
       <c r="M15">
         <v>265</v>
       </c>
-      <c r="N15" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N15">
+        <v>265</v>
+      </c>
+      <c r="O15">
+        <v>265</v>
+      </c>
+      <c r="P15">
+        <v>265</v>
+      </c>
+      <c r="Q15">
+        <v>265</v>
+      </c>
+      <c r="R15">
+        <v>265</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U15">
+        <v>13</v>
+      </c>
+      <c r="V15" t="s">
+        <v>86</v>
+      </c>
+      <c r="W15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1184,7 +1710,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1213,11 +1739,35 @@
       <c r="M16">
         <v>160</v>
       </c>
-      <c r="N16" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N16">
+        <v>160</v>
+      </c>
+      <c r="O16">
+        <v>160</v>
+      </c>
+      <c r="P16">
+        <v>160</v>
+      </c>
+      <c r="Q16">
+        <v>160</v>
+      </c>
+      <c r="R16">
+        <v>160</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U16">
+        <v>14</v>
+      </c>
+      <c r="V16" t="s">
+        <v>87</v>
+      </c>
+      <c r="W16">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1225,7 +1775,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1254,8 +1804,32 @@
       <c r="M17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>15</v>
+      </c>
+      <c r="V17" t="s">
+        <v>139</v>
+      </c>
+      <c r="W17">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1286,8 +1860,32 @@
       <c r="M18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>16</v>
+      </c>
+      <c r="V18" t="s">
+        <v>135</v>
+      </c>
+      <c r="W18">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1295,7 +1893,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19">
         <v>44</v>
@@ -1324,8 +1922,32 @@
       <c r="M19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>17</v>
+      </c>
+      <c r="V19" t="s">
+        <v>136</v>
+      </c>
+      <c r="W19">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1333,7 +1955,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20">
         <v>70</v>
@@ -1362,16 +1984,40 @@
       <c r="M20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>18</v>
+      </c>
+      <c r="V20" t="s">
+        <v>137</v>
+      </c>
+      <c r="W20">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21">
         <v>108</v>
@@ -1400,8 +2046,32 @@
       <c r="M21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>19</v>
+      </c>
+      <c r="V21" t="s">
+        <v>138</v>
+      </c>
+      <c r="W21">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1432,13 +2102,31 @@
       <c r="M22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1467,19 +2155,37 @@
       <c r="M23">
         <v>44</v>
       </c>
-      <c r="N23" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N23">
+        <v>44</v>
+      </c>
+      <c r="O23">
+        <v>44</v>
+      </c>
+      <c r="P23">
+        <v>44</v>
+      </c>
+      <c r="Q23">
+        <v>44</v>
+      </c>
+      <c r="R23">
+        <v>44</v>
+      </c>
+      <c r="S23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="U23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1508,8 +2214,26 @@
       <c r="M24">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N24">
+        <v>25</v>
+      </c>
+      <c r="O24">
+        <v>25</v>
+      </c>
+      <c r="P24">
+        <v>25</v>
+      </c>
+      <c r="Q24">
+        <v>25</v>
+      </c>
+      <c r="R24">
+        <v>25</v>
+      </c>
+      <c r="U24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1540,8 +2264,26 @@
       <c r="M25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1575,8 +2317,26 @@
       <c r="M26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1607,11 +2367,29 @@
       <c r="M27">
         <v>12593</v>
       </c>
-      <c r="N27" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N27">
+        <v>12593</v>
+      </c>
+      <c r="O27">
+        <v>12593</v>
+      </c>
+      <c r="P27">
+        <v>12593</v>
+      </c>
+      <c r="Q27">
+        <v>12593</v>
+      </c>
+      <c r="R27">
+        <v>12593</v>
+      </c>
+      <c r="S27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="U27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1642,11 +2420,29 @@
       <c r="M28">
         <v>12593</v>
       </c>
-      <c r="N28" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N28">
+        <v>12593</v>
+      </c>
+      <c r="O28">
+        <v>12593</v>
+      </c>
+      <c r="P28">
+        <v>12593</v>
+      </c>
+      <c r="Q28">
+        <v>12593</v>
+      </c>
+      <c r="R28">
+        <v>12593</v>
+      </c>
+      <c r="S28" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="U28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1677,11 +2473,29 @@
       <c r="M29">
         <v>12593</v>
       </c>
-      <c r="N29" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N29">
+        <v>12593</v>
+      </c>
+      <c r="O29">
+        <v>12593</v>
+      </c>
+      <c r="P29">
+        <v>12593</v>
+      </c>
+      <c r="Q29">
+        <v>12593</v>
+      </c>
+      <c r="R29">
+        <v>12593</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="U29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1689,7 +2503,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -1718,8 +2532,26 @@
       <c r="M30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1727,7 +2559,7 @@
         <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1756,8 +2588,26 @@
       <c r="M31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1765,7 +2615,7 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1794,8 +2644,26 @@
       <c r="M32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1803,7 +2671,7 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1832,8 +2700,26 @@
       <c r="M33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1841,7 +2727,7 @@
         <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -1870,8 +2756,26 @@
       <c r="M34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1902,8 +2806,26 @@
       <c r="M35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1934,8 +2856,26 @@
       <c r="M36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1966,8 +2906,26 @@
       <c r="M37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="U37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1998,8 +2956,26 @@
       <c r="M38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2030,8 +3006,26 @@
       <c r="M39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="U39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2062,8 +3056,26 @@
       <c r="M40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2094,8 +3106,26 @@
       <c r="M41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="U41">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2126,8 +3156,26 @@
       <c r="M42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="U42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2158,8 +3206,26 @@
       <c r="M43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+      <c r="U43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2190,8 +3256,26 @@
       <c r="M44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="U44">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2222,8 +3306,26 @@
       <c r="M45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="U45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2254,8 +3356,29 @@
       <c r="M46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="U46">
+        <v>44</v>
+      </c>
+      <c r="V46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2286,8 +3409,29 @@
       <c r="M47">
         <v>600</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N47">
+        <v>600</v>
+      </c>
+      <c r="O47">
+        <v>600</v>
+      </c>
+      <c r="P47">
+        <v>600</v>
+      </c>
+      <c r="Q47">
+        <v>600</v>
+      </c>
+      <c r="R47">
+        <v>600</v>
+      </c>
+      <c r="U47">
+        <v>45</v>
+      </c>
+      <c r="V47" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2318,8 +3462,26 @@
       <c r="M48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="U48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2350,8 +3512,26 @@
       <c r="M49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="U49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2382,8 +3562,26 @@
       <c r="M50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+      <c r="R50">
+        <v>0</v>
+      </c>
+      <c r="U50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2414,8 +3612,26 @@
       <c r="M51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+      <c r="R51">
+        <v>0</v>
+      </c>
+      <c r="U51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2446,8 +3662,26 @@
       <c r="M52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="P52">
+        <v>0</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+      <c r="U52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2478,8 +3712,26 @@
       <c r="M53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
+      </c>
+      <c r="U53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2510,8 +3762,26 @@
       <c r="M54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N54">
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="Q54">
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+      <c r="U54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2542,8 +3812,26 @@
       <c r="M55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+      <c r="Q55">
+        <v>0</v>
+      </c>
+      <c r="R55">
+        <v>0</v>
+      </c>
+      <c r="U55">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2574,8 +3862,26 @@
       <c r="M56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+      <c r="P56">
+        <v>0</v>
+      </c>
+      <c r="Q56">
+        <v>0</v>
+      </c>
+      <c r="R56">
+        <v>0</v>
+      </c>
+      <c r="U56">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2606,8 +3912,26 @@
       <c r="M57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N57">
+        <v>0</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="P57">
+        <v>0</v>
+      </c>
+      <c r="Q57">
+        <v>0</v>
+      </c>
+      <c r="R57">
+        <v>0</v>
+      </c>
+      <c r="U57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2638,8 +3962,26 @@
       <c r="M58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58">
+        <v>0</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+      <c r="Q58">
+        <v>0</v>
+      </c>
+      <c r="R58">
+        <v>0</v>
+      </c>
+      <c r="U58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -2670,8 +4012,26 @@
       <c r="M59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N59">
+        <v>0</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <v>0</v>
+      </c>
+      <c r="Q59">
+        <v>0</v>
+      </c>
+      <c r="R59">
+        <v>0</v>
+      </c>
+      <c r="U59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -2702,8 +4062,26 @@
       <c r="M60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N60">
+        <v>0</v>
+      </c>
+      <c r="O60">
+        <v>0</v>
+      </c>
+      <c r="P60">
+        <v>0</v>
+      </c>
+      <c r="Q60">
+        <v>0</v>
+      </c>
+      <c r="R60">
+        <v>0</v>
+      </c>
+      <c r="U60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -2734,8 +4112,26 @@
       <c r="M61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N61">
+        <v>0</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="Q61">
+        <v>0</v>
+      </c>
+      <c r="R61">
+        <v>0</v>
+      </c>
+      <c r="U61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -2766,8 +4162,26 @@
       <c r="M62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N62">
+        <v>0</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+      <c r="P62">
+        <v>0</v>
+      </c>
+      <c r="Q62">
+        <v>0</v>
+      </c>
+      <c r="R62">
+        <v>0</v>
+      </c>
+      <c r="U62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -2798,8 +4212,26 @@
       <c r="M63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N63">
+        <v>0</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <v>0</v>
+      </c>
+      <c r="R63">
+        <v>0</v>
+      </c>
+      <c r="U63">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -2830,8 +4262,26 @@
       <c r="M64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+      <c r="P64">
+        <v>0</v>
+      </c>
+      <c r="Q64">
+        <v>0</v>
+      </c>
+      <c r="R64">
+        <v>0</v>
+      </c>
+      <c r="U64">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -2862,8 +4312,26 @@
       <c r="M65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <v>0</v>
+      </c>
+      <c r="Q65">
+        <v>0</v>
+      </c>
+      <c r="R65">
+        <v>0</v>
+      </c>
+      <c r="U65">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -2894,8 +4362,26 @@
       <c r="M66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <v>0</v>
+      </c>
+      <c r="Q66">
+        <v>0</v>
+      </c>
+      <c r="R66">
+        <v>0</v>
+      </c>
+      <c r="U66">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -2903,7 +4389,7 @@
         <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -2932,8 +4418,26 @@
       <c r="M67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N67">
+        <v>0</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+      <c r="P67">
+        <v>0</v>
+      </c>
+      <c r="Q67">
+        <v>0</v>
+      </c>
+      <c r="R67">
+        <v>0</v>
+      </c>
+      <c r="U67">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -2941,7 +4445,7 @@
         <v>71</v>
       </c>
       <c r="C68" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D68">
         <v>4600</v>
@@ -2970,8 +4474,26 @@
       <c r="M68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N68">
+        <v>0</v>
+      </c>
+      <c r="O68">
+        <v>0</v>
+      </c>
+      <c r="P68">
+        <v>0</v>
+      </c>
+      <c r="Q68">
+        <v>0</v>
+      </c>
+      <c r="R68">
+        <v>0</v>
+      </c>
+      <c r="U68">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -2979,7 +4501,7 @@
         <v>72</v>
       </c>
       <c r="C69" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -3008,8 +4530,26 @@
       <c r="M69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <v>0</v>
+      </c>
+      <c r="P69">
+        <v>0</v>
+      </c>
+      <c r="Q69">
+        <v>0</v>
+      </c>
+      <c r="R69">
+        <v>0</v>
+      </c>
+      <c r="U69">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3017,7 +4557,7 @@
         <v>73</v>
       </c>
       <c r="C70" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D70">
         <v>70</v>
@@ -3046,8 +4586,26 @@
       <c r="M70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N70">
+        <v>0</v>
+      </c>
+      <c r="O70">
+        <v>0</v>
+      </c>
+      <c r="P70">
+        <v>0</v>
+      </c>
+      <c r="Q70">
+        <v>0</v>
+      </c>
+      <c r="R70">
+        <v>0</v>
+      </c>
+      <c r="U70">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -3057,8 +4615,26 @@
       <c r="M71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N71">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
+      <c r="R71">
+        <v>0</v>
+      </c>
+      <c r="U71">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -3068,8 +4644,29 @@
       <c r="M72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N72">
+        <v>0</v>
+      </c>
+      <c r="O72">
+        <v>0</v>
+      </c>
+      <c r="P72">
+        <v>0</v>
+      </c>
+      <c r="Q72">
+        <v>0</v>
+      </c>
+      <c r="R72">
+        <v>0</v>
+      </c>
+      <c r="U72">
+        <v>70</v>
+      </c>
+      <c r="V72" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -3079,11 +4676,32 @@
       <c r="M73">
         <v>4600</v>
       </c>
-      <c r="N73" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N73">
+        <v>4600</v>
+      </c>
+      <c r="O73">
+        <v>4600</v>
+      </c>
+      <c r="P73">
+        <v>4600</v>
+      </c>
+      <c r="Q73">
+        <v>4600</v>
+      </c>
+      <c r="R73">
+        <v>4600</v>
+      </c>
+      <c r="S73" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U73">
+        <v>71</v>
+      </c>
+      <c r="V73" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
@@ -3093,8 +4711,29 @@
       <c r="M74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N74">
+        <v>0</v>
+      </c>
+      <c r="O74">
+        <v>0</v>
+      </c>
+      <c r="P74">
+        <v>0</v>
+      </c>
+      <c r="Q74">
+        <v>0</v>
+      </c>
+      <c r="R74">
+        <v>0</v>
+      </c>
+      <c r="U74">
+        <v>72</v>
+      </c>
+      <c r="V74" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -3104,13 +4743,31 @@
       <c r="M75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N75">
+        <v>0</v>
+      </c>
+      <c r="O75">
+        <v>0</v>
+      </c>
+      <c r="P75">
+        <v>0</v>
+      </c>
+      <c r="Q75">
+        <v>0</v>
+      </c>
+      <c r="R75">
+        <v>0</v>
+      </c>
+      <c r="U75">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
       <c r="C76" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K76">
         <v>0</v>
@@ -3118,8 +4775,26 @@
       <c r="M76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N76">
+        <v>0</v>
+      </c>
+      <c r="O76">
+        <v>0</v>
+      </c>
+      <c r="P76">
+        <v>0</v>
+      </c>
+      <c r="Q76">
+        <v>0</v>
+      </c>
+      <c r="R76">
+        <v>0</v>
+      </c>
+      <c r="U76">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -3127,7 +4802,7 @@
         <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K77">
         <v>0</v>
@@ -3135,8 +4810,26 @@
       <c r="M77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N77">
+        <v>0</v>
+      </c>
+      <c r="O77">
+        <v>0</v>
+      </c>
+      <c r="P77">
+        <v>0</v>
+      </c>
+      <c r="Q77">
+        <v>0</v>
+      </c>
+      <c r="R77">
+        <v>0</v>
+      </c>
+      <c r="U77">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -3144,7 +4837,7 @@
         <v>82</v>
       </c>
       <c r="C78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K78">
         <v>16</v>
@@ -3152,8 +4845,29 @@
       <c r="M78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N78">
+        <v>0</v>
+      </c>
+      <c r="O78">
+        <v>0</v>
+      </c>
+      <c r="P78">
+        <v>0</v>
+      </c>
+      <c r="Q78">
+        <v>0</v>
+      </c>
+      <c r="R78">
+        <v>0</v>
+      </c>
+      <c r="U78">
+        <v>76</v>
+      </c>
+      <c r="V78" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -3163,45 +4877,246 @@
       <c r="M79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N79">
+        <v>1</v>
+      </c>
+      <c r="O79">
+        <v>1</v>
+      </c>
+      <c r="P79">
+        <v>1</v>
+      </c>
+      <c r="Q79">
+        <v>1</v>
+      </c>
+      <c r="R79">
+        <v>1</v>
+      </c>
+      <c r="U79">
+        <v>77</v>
+      </c>
+      <c r="V79" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>78</v>
+      </c>
       <c r="M80">
         <v>257</v>
       </c>
-    </row>
-    <row r="81" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="N80">
+        <v>257</v>
+      </c>
+      <c r="O80">
+        <v>257</v>
+      </c>
+      <c r="P80">
+        <v>257</v>
+      </c>
+      <c r="Q80">
+        <v>257</v>
+      </c>
+      <c r="R80">
+        <v>257</v>
+      </c>
+      <c r="U80">
+        <v>78</v>
+      </c>
+      <c r="V80" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>79</v>
+      </c>
       <c r="M81">
         <v>2</v>
       </c>
-    </row>
-    <row r="82" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="N81">
+        <v>2</v>
+      </c>
+      <c r="O81">
+        <v>2</v>
+      </c>
+      <c r="P81">
+        <v>1</v>
+      </c>
+      <c r="Q81">
+        <v>1</v>
+      </c>
+      <c r="R81">
+        <v>1</v>
+      </c>
+      <c r="U81">
+        <v>79</v>
+      </c>
+      <c r="V81" t="s">
+        <v>134</v>
+      </c>
+      <c r="W81">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>80</v>
+      </c>
       <c r="M82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="N82">
+        <v>0</v>
+      </c>
+      <c r="O82">
+        <v>0</v>
+      </c>
+      <c r="P82">
+        <v>0</v>
+      </c>
+      <c r="Q82">
+        <v>0</v>
+      </c>
+      <c r="R82">
+        <v>0</v>
+      </c>
+      <c r="U82">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>81</v>
+      </c>
       <c r="M83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="N83">
+        <v>0</v>
+      </c>
+      <c r="O83">
+        <v>0</v>
+      </c>
+      <c r="P83">
+        <v>0</v>
+      </c>
+      <c r="Q83">
+        <v>1</v>
+      </c>
+      <c r="R83">
+        <v>2</v>
+      </c>
+      <c r="S83" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U83">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>82</v>
+      </c>
       <c r="M84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="N84">
+        <v>0</v>
+      </c>
+      <c r="O84">
+        <v>0</v>
+      </c>
+      <c r="P84">
+        <v>0</v>
+      </c>
+      <c r="Q84">
+        <v>0</v>
+      </c>
+      <c r="R84">
+        <v>0</v>
+      </c>
+      <c r="U84">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>83</v>
+      </c>
       <c r="M85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="N85">
+        <v>0</v>
+      </c>
+      <c r="O85">
+        <v>0</v>
+      </c>
+      <c r="P85">
+        <v>0</v>
+      </c>
+      <c r="Q85">
+        <v>0</v>
+      </c>
+      <c r="R85">
+        <v>0</v>
+      </c>
+      <c r="U85">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>84</v>
+      </c>
       <c r="M86">
         <v>220</v>
       </c>
-    </row>
-    <row r="87" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="N86">
+        <v>220</v>
+      </c>
+      <c r="O86">
+        <v>220</v>
+      </c>
+      <c r="P86">
+        <v>220</v>
+      </c>
+      <c r="Q86">
+        <v>220</v>
+      </c>
+      <c r="R86">
+        <v>220</v>
+      </c>
+      <c r="U86">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>85</v>
+      </c>
       <c r="M87">
         <v>0</v>
+      </c>
+      <c r="N87">
+        <v>0</v>
+      </c>
+      <c r="O87">
+        <v>0</v>
+      </c>
+      <c r="P87">
+        <v>0</v>
+      </c>
+      <c r="Q87">
+        <v>0</v>
+      </c>
+      <c r="R87">
+        <v>0</v>
+      </c>
+      <c r="U87">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3212,34 +5127,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8C0C25-584C-4DB3-91C9-D576A78C1B11}">
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="8" max="8" width="10.77734375" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3261,11 +5176,14 @@
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3287,13 +5205,16 @@
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4">
         <v>23488</v>
@@ -3313,13 +5234,16 @@
       <c r="J4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>23535</v>
@@ -3336,16 +5260,19 @@
       <c r="H5">
         <v>23382</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6">
         <v>23606</v>
@@ -3362,16 +5289,19 @@
       <c r="H6">
         <v>23225</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -3388,16 +5318,19 @@
       <c r="H7">
         <v>23300</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -3414,16 +5347,19 @@
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -3440,16 +5376,19 @@
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -3466,16 +5405,19 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -3492,16 +5434,19 @@
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -3518,11 +5463,14 @@
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3544,16 +5492,19 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -3570,11 +5521,14 @@
       <c r="H14">
         <v>0</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3593,13 +5547,16 @@
       <c r="H15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16">
         <v>196</v>
@@ -3616,13 +5573,16 @@
       <c r="H16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -3639,11 +5599,14 @@
       <c r="H17">
         <v>4</v>
       </c>
-      <c r="J17" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3665,11 +5628,14 @@
       <c r="H18">
         <v>0</v>
       </c>
-      <c r="J18" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3691,8 +5657,11 @@
       <c r="H19">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3714,8 +5683,11 @@
       <c r="H20">
         <v>65527</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3737,8 +5709,11 @@
       <c r="H21">
         <v>65528</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3760,8 +5735,11 @@
       <c r="H22">
         <v>65534</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3783,13 +5761,16 @@
       <c r="H23">
         <v>65535</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C24">
         <v>65395</v>
@@ -3806,8 +5787,11 @@
       <c r="H24">
         <v>65535</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K24" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3829,8 +5813,11 @@
       <c r="H25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3852,11 +5839,14 @@
       <c r="H26">
         <v>15</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="J26" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3875,11 +5865,14 @@
       <c r="H27">
         <v>21</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="J27" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3901,8 +5894,11 @@
       <c r="H28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K28" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3921,8 +5917,11 @@
       <c r="H29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K29" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3941,8 +5940,11 @@
       <c r="H30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K30" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3961,8 +5963,11 @@
       <c r="H31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K31" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3981,8 +5986,11 @@
       <c r="H32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K32" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -4001,8 +6009,11 @@
       <c r="H33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K33" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -4021,13 +6032,16 @@
       <c r="H34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K34" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C35">
         <v>4992</v>
@@ -4044,16 +6058,19 @@
       <c r="H35">
         <v>4984</v>
       </c>
-      <c r="J35" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J35" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C36">
         <v>4984</v>
@@ -4070,16 +6087,19 @@
       <c r="H36">
         <v>4988</v>
       </c>
-      <c r="J36" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C37">
         <v>4996</v>
@@ -4096,16 +6116,19 @@
       <c r="H37">
         <v>4984</v>
       </c>
-      <c r="J37" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38">
         <v>549</v>
@@ -4122,16 +6145,19 @@
       <c r="H38">
         <v>13074</v>
       </c>
-      <c r="J38" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39">
         <v>5643</v>
@@ -4148,16 +6174,19 @@
       <c r="H39">
         <v>1810</v>
       </c>
-      <c r="J39" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40">
         <v>5899</v>
@@ -4174,11 +6203,14 @@
       <c r="H40">
         <v>6155</v>
       </c>
-      <c r="J40" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J40" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -4198,8 +6230,11 @@
       <c r="H41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K41" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -4219,7 +6254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -4239,7 +6274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -4259,7 +6294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -4279,7 +6314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -4299,7 +6334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -4319,7 +6354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -4339,7 +6374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -4359,10 +6394,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
+      <c r="B50" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="C50">
         <v>1</v>
       </c>
@@ -4378,8 +6416,11 @@
       <c r="H50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K50" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -4398,8 +6439,11 @@
       <c r="H51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K51" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -4418,8 +6462,11 @@
       <c r="H52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K52" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -4438,8 +6485,11 @@
       <c r="H53">
         <v>1338</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K53" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -4458,8 +6508,11 @@
       <c r="H54">
         <v>1301</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K54" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -4478,8 +6531,11 @@
       <c r="H55">
         <v>6153</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K55" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -4498,8 +6554,11 @@
       <c r="H56">
         <v>48</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K56" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -4518,8 +6577,11 @@
       <c r="H57">
         <v>1195</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K57" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -4538,8 +6600,11 @@
       <c r="H58">
         <v>1000</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K58" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -4558,8 +6623,11 @@
       <c r="H59">
         <v>60</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K59" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -4578,8 +6646,11 @@
       <c r="H60">
         <v>49</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K60" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -4598,8 +6669,11 @@
       <c r="H61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K61" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -4618,8 +6692,11 @@
       <c r="H62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K62" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -4638,8 +6715,11 @@
       <c r="H63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K63" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -4658,8 +6738,11 @@
       <c r="H64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K64" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -4678,8 +6761,11 @@
       <c r="H65">
         <v>100</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K65" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -4698,8 +6784,11 @@
       <c r="H66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K66" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -4718,8 +6807,11 @@
       <c r="H67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K67" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -4738,8 +6830,11 @@
       <c r="H68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K68" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -4758,8 +6853,11 @@
       <c r="H69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K69" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -4778,8 +6876,11 @@
       <c r="H70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K70" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -4798,8 +6899,11 @@
       <c r="H71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K71" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -4818,8 +6922,11 @@
       <c r="H72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K72" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -4838,8 +6945,11 @@
       <c r="H73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K73" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
@@ -4858,8 +6968,11 @@
       <c r="H74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K74" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -4878,8 +6991,11 @@
       <c r="H75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K75" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -4899,7 +7015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -4919,7 +7035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -4939,7 +7055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -4959,7 +7075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
@@ -5050,7 +7166,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C84">
         <v>12318</v>
@@ -5073,7 +7189,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C85">
         <v>5141</v>
@@ -5096,7 +7212,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C86">
         <v>5899</v>
@@ -5118,8 +7234,8 @@
       <c r="A87">
         <v>85</v>
       </c>
-      <c r="B87" t="s">
-        <v>14</v>
+      <c r="B87" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -5162,7 +7278,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -5185,7 +7301,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C90">
         <v>1</v>
@@ -5208,7 +7324,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -5230,6 +7346,9 @@
       <c r="A92">
         <v>90</v>
       </c>
+      <c r="B92" s="6" t="s">
+        <v>130</v>
+      </c>
       <c r="C92">
         <v>0</v>
       </c>
@@ -5251,7 +7370,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C93">
         <v>120</v>
@@ -5274,7 +7393,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C94">
         <v>1195</v>
@@ -5297,7 +7416,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C95">
         <v>1000</v>
@@ -5340,7 +7459,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C97">
         <v>44</v>

</xml_diff>

<commit_message>
#60 - API alows only 10 chars password length
</commit_message>
<xml_diff>
--- a/doc/Mapping.xlsx
+++ b/doc/Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trest\Source\Repos\HomeAssistant\homeassistant-solax-http\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60824D9-C86F-4332-AC91-FA0805E9BD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DA7FF2-E85A-494D-A251-565FBD2D43D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E30620CE-52E2-4698-983C-BDD3AD23A8BB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="146">
   <si>
     <t>[</t>
   </si>
@@ -457,6 +457,24 @@
   </si>
   <si>
     <t>boostMode</t>
+  </si>
+  <si>
+    <t>MainBreakerLimitSwitch</t>
+  </si>
+  <si>
+    <t>UserSetMaxCurrent</t>
+  </si>
+  <si>
+    <t>autoPhaseValue</t>
+  </si>
+  <si>
+    <t>SlaveAddress</t>
+  </si>
+  <si>
+    <t>SalveBraudRate</t>
+  </si>
+  <si>
+    <t>cableLockValue</t>
   </si>
 </sst>
 </file>
@@ -853,7 +871,7 @@
   <dimension ref="A1:W87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2:W21"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1074,6 +1092,9 @@
       <c r="U4">
         <v>2</v>
       </c>
+      <c r="V4" s="6" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -1254,6 +1275,12 @@
       <c r="U7">
         <v>5</v>
       </c>
+      <c r="V7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="W7">
+        <v>56</v>
+      </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -1359,6 +1386,9 @@
       </c>
       <c r="U9">
         <v>7</v>
+      </c>
+      <c r="V9" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
@@ -1512,6 +1542,9 @@
       <c r="U12" s="1">
         <v>10</v>
       </c>
+      <c r="V12" s="6" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -2232,6 +2265,9 @@
       <c r="U24">
         <v>22</v>
       </c>
+      <c r="V24" s="6" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -2282,6 +2318,9 @@
       <c r="U25">
         <v>23</v>
       </c>
+      <c r="V25" s="6" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -2290,6 +2329,9 @@
       <c r="B26">
         <v>29</v>
       </c>
+      <c r="C26" t="s">
+        <v>134</v>
+      </c>
       <c r="D26">
         <v>0</v>
       </c>
@@ -4761,6 +4803,9 @@
       <c r="U75">
         <v>73</v>
       </c>
+      <c r="V75" s="6" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A76">
@@ -5117,6 +5162,9 @@
       </c>
       <c r="U87">
         <v>85</v>
+      </c>
+      <c r="V87" s="6" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -5127,20 +5175,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8C0C25-584C-4DB3-91C9-D576A78C1B11}">
-  <dimension ref="A1:K107"/>
+  <dimension ref="A1:M107"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" style="2" customWidth="1"/>
+    <col min="8" max="10" width="10.77734375" customWidth="1"/>
+    <col min="12" max="12" width="15.88671875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C1" s="4" t="s">
         <v>48</v>
       </c>
@@ -5154,7 +5202,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5176,14 +5224,20 @@
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
         <v>70</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5205,11 +5259,17 @@
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -5231,14 +5291,20 @@
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="M4" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -5260,14 +5326,20 @@
       <c r="H5">
         <v>23382</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="I5">
+        <v>22704</v>
+      </c>
+      <c r="J5">
+        <v>22546</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -5289,14 +5361,20 @@
       <c r="H6">
         <v>23225</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="I6">
+        <v>22408</v>
+      </c>
+      <c r="J6">
+        <v>22332</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -5318,14 +5396,20 @@
       <c r="H7">
         <v>23300</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="I7">
+        <v>22843</v>
+      </c>
+      <c r="J7">
+        <v>22795</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -5347,14 +5431,20 @@
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="I8">
+        <v>72</v>
+      </c>
+      <c r="J8">
+        <v>69</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -5376,14 +5466,20 @@
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -5405,14 +5501,20 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -5434,14 +5536,20 @@
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -5463,14 +5571,20 @@
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -5492,14 +5606,20 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -5521,14 +5641,20 @@
       <c r="H14">
         <v>0</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="M14" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -5547,11 +5673,17 @@
       <c r="H15">
         <v>0</v>
       </c>
-      <c r="K15" s="6" t="s">
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -5573,11 +5705,17 @@
       <c r="H16">
         <v>0</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="M16" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -5599,14 +5737,20 @@
       <c r="H17">
         <v>4</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="I17">
+        <v>1069</v>
+      </c>
+      <c r="J17">
+        <v>1071</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -5628,14 +5772,20 @@
       <c r="H18">
         <v>0</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -5657,11 +5807,17 @@
       <c r="H19">
         <v>11</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="I19">
+        <v>19</v>
+      </c>
+      <c r="J19">
+        <v>19</v>
+      </c>
+      <c r="M19" s="6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -5683,11 +5839,17 @@
       <c r="H20">
         <v>65527</v>
       </c>
-      <c r="K20" s="6" t="s">
+      <c r="I20">
+        <v>19</v>
+      </c>
+      <c r="J20">
+        <v>19</v>
+      </c>
+      <c r="M20" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -5709,11 +5871,17 @@
       <c r="H21">
         <v>65528</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="I21">
+        <v>65518</v>
+      </c>
+      <c r="J21">
+        <v>65518</v>
+      </c>
+      <c r="M21" s="6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -5735,11 +5903,17 @@
       <c r="H22">
         <v>65534</v>
       </c>
-      <c r="K22" s="6" t="s">
+      <c r="I22">
+        <v>78</v>
+      </c>
+      <c r="J22">
+        <v>65464</v>
+      </c>
+      <c r="M22" s="6" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -5761,11 +5935,17 @@
       <c r="H23">
         <v>65535</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="I23">
+        <v>30</v>
+      </c>
+      <c r="J23">
         <v>98</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M23" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -5787,11 +5967,17 @@
       <c r="H24">
         <v>65535</v>
       </c>
-      <c r="K24" s="6" t="s">
+      <c r="I24">
+        <v>7</v>
+      </c>
+      <c r="J24">
+        <v>16</v>
+      </c>
+      <c r="M24" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -5813,11 +5999,17 @@
       <c r="H25">
         <v>0</v>
       </c>
-      <c r="K25" s="6" t="s">
+      <c r="I25">
+        <v>417</v>
+      </c>
+      <c r="J25">
+        <v>471</v>
+      </c>
+      <c r="M25" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -5839,14 +6031,20 @@
       <c r="H26">
         <v>15</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="I26">
+        <v>13</v>
+      </c>
+      <c r="J26">
+        <v>14</v>
+      </c>
+      <c r="L26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="M26" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -5865,14 +6063,20 @@
       <c r="H27">
         <v>21</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="I27">
+        <v>20</v>
+      </c>
+      <c r="J27">
+        <v>20</v>
+      </c>
+      <c r="L27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="M27" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -5894,11 +6098,17 @@
       <c r="H28">
         <v>0</v>
       </c>
-      <c r="K28" s="6" t="s">
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="M28" s="6" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -5917,11 +6127,17 @@
       <c r="H29">
         <v>0</v>
       </c>
-      <c r="K29" s="6" t="s">
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="M29" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -5940,11 +6156,17 @@
       <c r="H30">
         <v>0</v>
       </c>
-      <c r="K30" s="6" t="s">
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="M30" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -5963,11 +6185,17 @@
       <c r="H31">
         <v>0</v>
       </c>
-      <c r="K31" s="6" t="s">
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="M31" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -5986,11 +6214,17 @@
       <c r="H32">
         <v>0</v>
       </c>
-      <c r="K32" s="6" t="s">
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="M32" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -6009,11 +6243,17 @@
       <c r="H33">
         <v>0</v>
       </c>
-      <c r="K33" s="6" t="s">
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="M33" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -6032,11 +6272,17 @@
       <c r="H34">
         <v>0</v>
       </c>
-      <c r="K34" s="6" t="s">
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="M34" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -6058,14 +6304,20 @@
       <c r="H35">
         <v>4984</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="I35">
+        <v>4988</v>
+      </c>
+      <c r="J35">
+        <v>4986</v>
+      </c>
+      <c r="L35" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="M35" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -6087,14 +6339,20 @@
       <c r="H36">
         <v>4988</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="I36">
+        <v>4984</v>
+      </c>
+      <c r="J36">
+        <v>4984</v>
+      </c>
+      <c r="L36" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K36" s="2" t="s">
+      <c r="M36" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -6116,14 +6374,20 @@
       <c r="H37">
         <v>4984</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="I37">
+        <v>4986</v>
+      </c>
+      <c r="J37">
+        <v>4986</v>
+      </c>
+      <c r="L37" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K37" s="2" t="s">
+      <c r="M37" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -6145,14 +6409,20 @@
       <c r="H38">
         <v>13074</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="I38">
+        <v>13366</v>
+      </c>
+      <c r="J38">
+        <v>14385</v>
+      </c>
+      <c r="L38" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="M38" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -6174,14 +6444,20 @@
       <c r="H39">
         <v>1810</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="I39">
+        <v>6414</v>
+      </c>
+      <c r="J39">
+        <v>6414</v>
+      </c>
+      <c r="L39" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K39" s="2" t="s">
+      <c r="M39" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -6203,14 +6479,20 @@
       <c r="H40">
         <v>6155</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="I40">
+        <v>6156</v>
+      </c>
+      <c r="J40">
+        <v>6156</v>
+      </c>
+      <c r="L40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K40" s="2" t="s">
+      <c r="M40" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -6230,11 +6512,17 @@
       <c r="H41">
         <v>4</v>
       </c>
-      <c r="K41" s="6" t="s">
+      <c r="I41">
+        <v>3</v>
+      </c>
+      <c r="J41">
+        <v>3</v>
+      </c>
+      <c r="M41" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -6253,8 +6541,14 @@
       <c r="H42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -6273,8 +6567,14 @@
       <c r="H43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -6293,8 +6593,14 @@
       <c r="H44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -6313,8 +6619,14 @@
       <c r="H45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -6333,8 +6645,14 @@
       <c r="H46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -6353,8 +6671,14 @@
       <c r="H47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -6373,8 +6697,14 @@
       <c r="H48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -6393,8 +6723,14 @@
       <c r="H49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -6416,11 +6752,17 @@
       <c r="H50">
         <v>1</v>
       </c>
-      <c r="K50" s="6" t="s">
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="M50" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -6439,11 +6781,17 @@
       <c r="H51">
         <v>0</v>
       </c>
-      <c r="K51" s="6" t="s">
+      <c r="I51">
+        <v>3</v>
+      </c>
+      <c r="J51">
+        <v>233</v>
+      </c>
+      <c r="M51" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -6462,11 +6810,17 @@
       <c r="H52">
         <v>0</v>
       </c>
-      <c r="K52" s="6" t="s">
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="M52" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -6485,11 +6839,17 @@
       <c r="H53">
         <v>1338</v>
       </c>
-      <c r="K53" s="6" t="s">
+      <c r="I53">
+        <v>13363</v>
+      </c>
+      <c r="J53">
+        <v>13363</v>
+      </c>
+      <c r="M53" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -6508,11 +6868,17 @@
       <c r="H54">
         <v>1301</v>
       </c>
-      <c r="K54" s="6" t="s">
+      <c r="I54">
+        <v>6414</v>
+      </c>
+      <c r="J54">
+        <v>6414</v>
+      </c>
+      <c r="M54" s="6" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -6531,11 +6897,17 @@
       <c r="H55">
         <v>6153</v>
       </c>
-      <c r="K55" s="6" t="s">
+      <c r="I55">
+        <v>6156</v>
+      </c>
+      <c r="J55">
+        <v>6156</v>
+      </c>
+      <c r="M55" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -6554,11 +6926,17 @@
       <c r="H56">
         <v>48</v>
       </c>
-      <c r="K56" s="6" t="s">
+      <c r="I56">
+        <v>48</v>
+      </c>
+      <c r="J56">
+        <v>48</v>
+      </c>
+      <c r="M56" s="6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -6577,11 +6955,17 @@
       <c r="H57">
         <v>1195</v>
       </c>
-      <c r="K57" s="6" t="s">
+      <c r="I57">
+        <v>565</v>
+      </c>
+      <c r="J57">
+        <v>596</v>
+      </c>
+      <c r="M57" s="6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -6600,11 +6984,17 @@
       <c r="H58">
         <v>1000</v>
       </c>
-      <c r="K58" s="6" t="s">
+      <c r="I58">
+        <v>166</v>
+      </c>
+      <c r="J58">
+        <v>1000</v>
+      </c>
+      <c r="M58" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -6623,11 +7013,17 @@
       <c r="H59">
         <v>60</v>
       </c>
-      <c r="K59" s="6" t="s">
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="M59" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -6646,11 +7042,17 @@
       <c r="H60">
         <v>49</v>
       </c>
-      <c r="K60" s="6" t="s">
+      <c r="I60">
+        <v>44</v>
+      </c>
+      <c r="J60">
+        <v>44</v>
+      </c>
+      <c r="M60" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -6669,11 +7071,17 @@
       <c r="H61">
         <v>0</v>
       </c>
-      <c r="K61" s="6" t="s">
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="M61" s="6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -6692,11 +7100,17 @@
       <c r="H62">
         <v>0</v>
       </c>
-      <c r="K62" s="6" t="s">
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="M62" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -6715,11 +7129,17 @@
       <c r="H63">
         <v>1</v>
       </c>
-      <c r="K63" s="6" t="s">
+      <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+      <c r="M63" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -6738,11 +7158,17 @@
       <c r="H64">
         <v>0</v>
       </c>
-      <c r="K64" s="6" t="s">
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="M64" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -6761,11 +7187,17 @@
       <c r="H65">
         <v>100</v>
       </c>
-      <c r="K65" s="6" t="s">
+      <c r="I65">
+        <v>100</v>
+      </c>
+      <c r="J65">
+        <v>100</v>
+      </c>
+      <c r="M65" s="6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -6784,11 +7216,17 @@
       <c r="H66">
         <v>0</v>
       </c>
-      <c r="K66" s="6" t="s">
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="M66" s="6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -6807,11 +7245,17 @@
       <c r="H67">
         <v>0</v>
       </c>
-      <c r="K67" s="6" t="s">
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="M67" s="6" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -6830,11 +7274,17 @@
       <c r="H68">
         <v>0</v>
       </c>
-      <c r="K68" s="6" t="s">
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="M68" s="6" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -6853,11 +7303,17 @@
       <c r="H69">
         <v>0</v>
       </c>
-      <c r="K69" s="6" t="s">
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="M69" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -6876,11 +7332,17 @@
       <c r="H70">
         <v>0</v>
       </c>
-      <c r="K70" s="6" t="s">
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="M70" s="6" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -6899,11 +7361,17 @@
       <c r="H71">
         <v>0</v>
       </c>
-      <c r="K71" s="6" t="s">
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="M71" s="6" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -6922,11 +7390,17 @@
       <c r="H72">
         <v>0</v>
       </c>
-      <c r="K72" s="6" t="s">
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="M72" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -6945,11 +7419,17 @@
       <c r="H73">
         <v>0</v>
       </c>
-      <c r="K73" s="6" t="s">
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="M73" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
@@ -6968,11 +7448,17 @@
       <c r="H74">
         <v>0</v>
       </c>
-      <c r="K74" s="6" t="s">
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="M74" s="6" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -6991,11 +7477,17 @@
       <c r="H75">
         <v>0</v>
       </c>
-      <c r="K75" s="6" t="s">
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="M75" s="6" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -7014,8 +7506,14 @@
       <c r="H76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -7034,8 +7532,14 @@
       <c r="H77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -7054,8 +7558,14 @@
       <c r="H78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -7074,8 +7584,14 @@
       <c r="H79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
@@ -7094,8 +7610,14 @@
       <c r="H80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
@@ -7114,8 +7636,14 @@
       <c r="H81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
@@ -7137,8 +7665,14 @@
       <c r="H82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I82">
+        <v>0</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
@@ -7160,8 +7694,14 @@
       <c r="H83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
@@ -7183,8 +7723,14 @@
       <c r="H84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -7206,8 +7752,14 @@
       <c r="H85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
@@ -7229,8 +7781,14 @@
       <c r="H86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
@@ -7252,8 +7810,14 @@
       <c r="H87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
@@ -7272,8 +7836,14 @@
       <c r="H88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
@@ -7295,8 +7865,14 @@
       <c r="H89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
@@ -7318,8 +7894,14 @@
       <c r="H90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="J90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
@@ -7341,8 +7923,14 @@
       <c r="H91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I91">
+        <v>0</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
@@ -7364,8 +7952,14 @@
       <c r="H92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I92">
+        <v>0</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
@@ -7387,8 +7981,14 @@
       <c r="H93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I93">
+        <v>0</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
@@ -7410,8 +8010,14 @@
       <c r="H94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I94">
+        <v>0</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
@@ -7433,8 +8039,14 @@
       <c r="H95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I95">
+        <v>0</v>
+      </c>
+      <c r="J95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
@@ -7453,8 +8065,14 @@
       <c r="H96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
@@ -7476,84 +8094,150 @@
       <c r="H97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F98">
         <v>0</v>
       </c>
       <c r="H98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I98">
+        <v>0</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F99">
         <v>0</v>
       </c>
       <c r="H99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I99">
+        <v>0</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F100">
         <v>1</v>
       </c>
       <c r="H100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I100">
+        <v>1</v>
+      </c>
+      <c r="J100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F101">
         <v>12</v>
       </c>
       <c r="H101">
         <v>13</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I101">
+        <v>12</v>
+      </c>
+      <c r="J101">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F102">
         <v>50</v>
       </c>
       <c r="H102">
         <v>50</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I102">
+        <v>50</v>
+      </c>
+      <c r="J102">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F103">
         <v>6</v>
       </c>
       <c r="H103">
         <v>5</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I103">
+        <v>34</v>
+      </c>
+      <c r="J103">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F104">
         <v>0</v>
       </c>
       <c r="H104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I104">
+        <v>0</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F105">
         <v>6</v>
       </c>
       <c r="H105">
         <v>5</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I105">
+        <v>24</v>
+      </c>
+      <c r="J105">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F106">
         <v>0</v>
       </c>
       <c r="H106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I106">
+        <v>0</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F107">
         <v>0</v>
       </c>
       <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="I107">
+        <v>0</v>
+      </c>
+      <c r="J107">
         <v>0</v>
       </c>
     </row>

</xml_diff>